<commit_message>
cleaning up bitcoin asset
</commit_message>
<xml_diff>
--- a/05-report-xlsx/report-template.xlsx
+++ b/05-report-xlsx/report-template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11219"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carendt/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nwstephens/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E725A0F-45AD-8A40-8627-E7C1177DD1EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="460" windowWidth="24660" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="1620" yWindow="460" windowWidth="24660" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitcoin Report" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,18 @@
   <definedNames>
     <definedName name="data" localSheetId="1">data!$A$1:$C$366</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,9 +40,9 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="data" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carendt/Downloads/data.csv" comma="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="data" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carendt/Downloads/data.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -89,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
@@ -223,12 +232,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -256,6 +259,12 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -267,3050 +276,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>last</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>data!$A$2:$A$366</c:f>
-              <c:numCache>
-                <c:formatCode>yyyy/mm/dd\ hh:mm:ss</c:formatCode>
-                <c:ptCount val="365"/>
-                <c:pt idx="0">
-                  <c:v>43189.0056944444</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43189.0157407407</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43189.0263888889</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43189.0368634259</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43189.0475115741</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43189.0578125</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43189.0681134259</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43189.0782986111</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43189.0890162037</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43189.0990625</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43189.1094791667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43189.120474537</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43189.1307175926</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43189.1412268518</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43189.1511226852</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43189.161724537</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43189.1720833333</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43189.1825578704</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43189.1928587963</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43189.2033449074</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43189.2141087963</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43189.2242824074</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43189.234537037</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43189.245462963</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>43189.2553009259</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43189.2662152778</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43189.2762268519</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>43189.2865856482</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>43189.2973611111</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43189.3079282407</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>43189.318287037</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>43189.3282986111</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43189.3387152778</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43189.349224537</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43189.3596990741</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>43189.3703472222</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>43189.3805439815</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>43189.3911111111</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43189.4015277778</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>43189.4118865741</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>43189.4221412037</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>43189.4329050926</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43189.442974537</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43189.453275463</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>43189.46375</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>43189.4742013889</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>43189.4850231481</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>43189.4950347222</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>43189.5052777778</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>43189.5159143519</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>43189.5261574074</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>43189.5366898148</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>43189.5474537037</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>43189.5574652778</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>43189.5678819444</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>43189.5784837963</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>43189.5887847222</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>43189.5992939815</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>43189.609537037</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>43189.6203587963</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>43189.6304398148</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>43189.6412384259</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>43189.65125</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>43189.6621296296</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>43189.6723726852</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>43189.6825462963</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>43189.6932523148</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>43189.7033796296</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>43189.7137384259</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>43189.724537037</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>43189.7350115741</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>43189.7451967593</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>43189.7553356482</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>43189.7659027778</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>43189.7764930556</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>43189.7870833333</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>43189.7973842593</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>43189.8075462963</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>43189.8180671296</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>43189.828599537</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>43189.8389583333</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>43189.8493518519</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>43189.8598263889</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>43189.869849537</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>43189.8804398148</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>43189.8907523148</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>43189.901400463</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>43189.9118171296</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>43189.922349537</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>43189.9326967593</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>43189.9429282407</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>43189.9536458333</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>43189.9637731481</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>43189.9741782407</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>43189.9848148148</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>43189.9951157407</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>43190.0058912037</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>43190.016099537</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>43190.0264814815</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>43190.0366087963</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>43190.0469791667</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>43190.0577199074</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>43190.0679050926</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>43190.0783333333</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>43190.0888657407</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>43190.0992013889</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>43190.1097337963</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>43190.1202083333</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>43190.1303356482</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>43190.1409027778</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>43190.1512615741</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>43190.1620833333</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>43190.1722222222</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>43190.1825231481</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>43190.1928819444</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>43190.203587963</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>43190.2137731481</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>43190.2241087963</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>43190.2348148148</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>43190.2452893518</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>43190.2556018519</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>43190.2661342593</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>43190.2763773148</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>43190.2869097222</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>43190.2970023148</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>43190.3077777778</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>43190.3179166667</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>43190.3282175926</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>43190.33875</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>43190.3494560185</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>43190.3598148148</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>43190.3703472222</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>43190.3803587963</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>43190.3908101852</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>43190.4012847222</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>43190.4120023148</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>43190.4219560185</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>43190.4327777778</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>43190.4431365741</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>43190.4533217593</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>43190.4636805556</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>43190.4740277778</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>43190.4847337963</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>43190.4952662037</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>43190.5055671296</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>43190.5159143519</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>43190.5261574074</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>43190.5366319444</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>43190.5469907407</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>43190.5573842593</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>43190.5682638889</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>43190.5785185185</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>43190.5889814815</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>43190.5990972222</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>43190.6098611111</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>43190.6198726852</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>43190.6302893519</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>43190.6408564815</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>43190.6514467593</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>43190.6619212963</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>43190.6722800926</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>43190.6827546296</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>43190.6928240741</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>43190.7033564815</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>43190.7137152778</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>43190.7245833333</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>43190.7348842593</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>43190.7453009259</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>43190.7556018519</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>43190.7657291667</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>43190.7763194444</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>43190.7868518519</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>43190.7971643519</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>43190.8077662037</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>43190.8182175926</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>43190.8282986111</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>43190.8387731481</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>43190.8491087963</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>43190.8597569444</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>43190.87</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>43190.8806481481</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>43190.8913310185</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>43190.9017013889</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>43190.9118402778</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>43190.9222453704</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>43190.9325347222</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>43190.943125</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>43190.9538425926</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>43190.9640740741</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>43190.9745023148</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>43190.984525463</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>43190.995</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>43191.0053587963</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>43191.0159722222</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>43191.0264467593</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>43191.0368634259</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>43191.047337963</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>43191.0579050926</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>43191.0681481481</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>43191.078275463</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>43191.0890509259</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>43191.0994444444</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>43191.1100347222</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>43191.1200462963</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>43191.1303587963</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>43191.1410069444</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>43191.15125</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>43191.1616666667</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>43191.1724884259</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>43191.1827777778</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>43191.1931944444</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>43191.2037268518</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>43191.2138541667</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>43191.224212963</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>43191.2349305556</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>43191.2452314815</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>43191.255474537</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>43191.2657523148</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>43191.2762847222</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>43191.2869328704</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>43191.2971180556</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>43191.3075231481</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>43191.3180555556</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>43191.328587963</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>43191.3386574074</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>43191.3495138889</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>43191.3599305556</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>43191.37</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>43191.3806481481</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>43191.3911111111</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>43191.401412037</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>43191.4121759259</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>43191.4223032407</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>43191.4324421296</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>43191.4430902778</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>43191.4536226852</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>43191.4640393518</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>43191.4745717593</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>43191.4844791667</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>43191.4950115741</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>43191.5054282407</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>43191.5163078704</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>43191.5262037037</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>43191.5365740741</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>43191.5471643519</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>43191.5575</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>43191.5678703704</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>43191.5783449074</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>43191.5887037037</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>43191.5995023148</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>43191.6096296296</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>43191.6201736111</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>43191.630474537</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>43191.6408796296</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>43191.6513541667</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>43191.6617708333</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>43191.6721875</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>43191.6824305556</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>43191.692962963</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>43191.7034375</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>43191.7139236111</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>43191.7241550926</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>43191.7346875</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>43191.7452199074</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>43191.755462963</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>43191.7660416667</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>43191.7762268519</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>43191.7868171296</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>43191.7972337963</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>43191.8079166667</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>43191.8183333333</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>43191.8282986111</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>43191.8387731481</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>43191.8491319444</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>43191.8596064815</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>43191.8700925926</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>43191.8806828704</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>43191.8909143519</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>43191.9016203704</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>43191.9116898148</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>43191.9220486111</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>43191.9325347222</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>43191.9428356482</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>43191.9533217593</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>43191.9640162037</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>43191.9744328704</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>43191.9847337963</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>43191.9952083333</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>43192.0055787037</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>43192.015787037</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>43192.0261574074</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>43192.0365740741</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>43192.0470486111</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>43192.0576851852</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>43192.0678703704</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>43192.07875</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>43192.0888194444</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>43192.099224537</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>43192.1098726852</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>43192.1203472222</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>43192.1305902778</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>43192.1408101852</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>43192.151412037</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>43192.1620023148</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>43192.1723032407</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>43192.1827546296</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>43192.1931134259</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>43192.2035300926</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>43192.2138310185</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>43192.224375</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>43192.2350810185</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>43192.2450347222</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>43192.2554513889</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>43192.2661574074</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>43192.2762962963</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>43192.2871180556</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>43192.2973032407</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>43192.3077777778</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>43192.3177893519</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>43192.3283796296</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>43192.3389699074</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>43192.3492013889</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>43192.3596180556</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>43192.3699189815</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>43192.3803935185</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>43192.3909143519</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>43192.4015046296</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>43192.4118055556</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>43192.4225694444</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>43192.4323958333</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>43192.4433333333</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>43192.453287037</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>43192.4637615741</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>43192.4740393519</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>43192.484525463</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>43192.4950578704</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>43192.5053587963</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>43192.5159490741</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>43192.5261921296</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>43192.5367824074</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>43192.5473958333</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>43192.5576736111</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>43192.5682638889</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>43192.5783333333</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>43192.5889236111</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>43192.5995138889</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>43192.6098148148</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>43192.6200578704</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>43192.6304976852</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>43192.6407986111</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>43192.651099537</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>43192.6619212963</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>43192.6722800926</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>43192.6823958333</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>43192.6928125</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>43192.7032291667</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>43192.7138773148</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>43192.7245949074</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>43192.7346064815</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>43192.7449189815</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>43192.7554282407</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>43192.7658217593</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>43192.7761226852</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>43192.7866666667</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>43192.7974884259</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$B$2:$B$366</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="365"/>
-                <c:pt idx="0">
-                  <c:v>7130.27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7066.97</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6893.1068696</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6948.94</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6811.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6730.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6878.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6888.47</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6923.33</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6846.5658007</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6851.83</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6833.61</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6873.349113</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6834.93</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6908.13</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6889.81</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6830.27</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6720.06</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6693.24</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6707.3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6786.7951995</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6769.78</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6965.41</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7103.58</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7082.82</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7147.62</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7131.66</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7088.44</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6977.99</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7060.65</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7114.56</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7236.4703964</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7264.53</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7224.43</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7213.2517116</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7150.33</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7117.3411645</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>7130.96</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7126.93</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7087.37</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7058.76</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>7087.83</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>7053.7219973</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>6953.02</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>6946.11</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>6978.4133692</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>6954.69</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>7034.2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>6958.27</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6974.15</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>7034.77</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>7006.56</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>7046.6290541</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6990.14</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6847.51</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6892.85</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>6915.56</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6939.67</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>6913.3504748</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>6882.58</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6814.24</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6746.352229</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6745.14</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6743.06</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6784.03</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6731.74</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6765.8012768</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6628.09</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6698.38</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6642.5</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>6704.8041604</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>6681.11</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>6749.66</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>6693.77</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>6723.76</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>6754.0201513</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>6808.96</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>6767.46</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>6845.44</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>6819.51</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>6809.54</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>6823.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>6819.79</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>6883.41</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>6857.32</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>6897.22</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>6919.17</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>6945.04</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>6895.59</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>6891.71</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>6772.74</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>6779.7217728</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>6814.78</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>6819.2</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>6839.46</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>6861.83</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>6896.85</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>7005.41</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>6986.31</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>7017.49</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>6965.78</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>7023.27</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>7048.51</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>7058.14</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>7098.49</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>7055.8159628</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>7044.59</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>7049.7</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>7005.43</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>7033.14</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>7052.26</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>7019.42</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>7006.03</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>7025.63</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>7049.92</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>7046.02</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>7006.14</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>7005.6640525</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>6930.46</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>6906.86</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>6913.3</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>6920.14</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>6905.33</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>6831.29</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>6830.22</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>6833.12</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>6838.18</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>6855.12</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>6847.98</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>6903.0641543</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>6932.8978368</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>6931.27</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>6905.55</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>6889.36</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>6915.08</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>7001.57</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7018.8078653</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>7009.63</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>7126.81</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>7167.56</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>7122.21</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>7070.29</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>7103.61</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>7124.09</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>7128.13</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>7126.68</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>7138.77</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>7195.39</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>7152.79</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>7130.37</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>7105.61</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>7071.64</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>7075.35</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>7026.956835</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>7009.85</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7045.21</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>7036.9601133</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>7046.41</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>7074.24</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>7062.2007253</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>7114.69</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>7155.92</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>7126.06</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>7154.25</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>7165.56</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>7109.76</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>7077.51</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>7093.9</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>7102.74</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>7105.5343061</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>7080.93</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>7047.1</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>7057.04</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>7036.01</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>7044.14</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>7045.54</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>7068.37</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>7001.11</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>6911.83</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>6934.32</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>6931.35</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>6906.7252521</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>6936.52</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>6950.0730516</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>6943.03</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>6955.49</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>6961.88</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>6964.34</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>6967.9</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>6908.5487694</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>6931.3640964</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>6937.69</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>7006.95</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>7015.5225986</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>7015.64</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>6994.74</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>7004.8</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>7014.69</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>7027.4744965</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>7031.97</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>6999.24</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>7013.98</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>6977.98</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>6944.9404194</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>6949.86</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>6931.16</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>6959.02</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>6954.22</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>6944.37</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>6979.06</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>6965.89</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>6945.73</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>6950.86</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>6953.56</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>6943.96</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>6939.87</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>6881.57</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>6885.76</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>6860.8070662</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>6862.67</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>6849.75</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>6783.34</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>6714.73</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>6719.1139069</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>6743.9</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>6729.71</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>6716.872463</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>6724.75</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>6675.45</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>6684.12</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>6701.74</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>6730.63</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>6747.62</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>6722.17</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>6702.0732913</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>6716.14</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>6709.49</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>6705.9</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>6693.56</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>6714.91</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>6729.43</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>6737.52</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>6710.84</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>6718.54</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>6704.94</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>6644.55438</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>6590.78</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>6609.68</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>6515.7</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>6509.4176573</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>6493.16</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>6512.16</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>6532.84</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>6535.21</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>6513.0656359</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>6504.77</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>6523.4</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>6765.89</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>6842.46</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>6861.75</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>6813.53</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>6850.6</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>6813.64</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>6874.34</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>6862.2</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>6843.3174957</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>6767.11</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>6773.13</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>6839.11</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>6924.66</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>6968.84</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>6948.58</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>6904.04</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>6903.02</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>6939.57</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>6924.46</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>6886.52</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>6905.95</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>6847.54</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>6844.9895907</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>6856.34</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>6825.65</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>6785.11</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>6811.2</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>6792.17</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>6835.56</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>6794.79</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>6827.86</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>6798.1474429</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>6798.33</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>6807.31</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>7011.48</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>6971.73</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>6997.21</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>7003.94</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>6973.616238</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>6967.47</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>6959.24</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>6977.21</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>6964.37</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>6984.57</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>6967.03</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>6981.13</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>6974.3</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>7022.84</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>6967.01</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>6959.52</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>6905.92</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>6874.94</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>6900.61</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>6912.3</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>6922.45</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>6927.0</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>6955.03</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>6943.64</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>6918.31</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>6904.8790713</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>6947.6</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>6959.04</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>7034.94</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>7099.21</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>7058.98</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>7045.0917075</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>7061.34</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>7077.4087542</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>7086.72</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>7068.99</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>7074.56</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>7071.4195118</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>7033.0698941</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>7048.19</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>7076.95</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>7058.11</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>7097.15</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>7095.85</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>7071.0</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>7055.09</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>7043.6344418</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>7010.62</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>7033.41</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>7027.1895352</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>7034.88</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>7038.66</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>7014.99</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>7017.09</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>6935.5</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>6919.56</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>6940.47</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>6950.8537859</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>6949.83</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>7016.9846766</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>7047.3547226</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>7039.43</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>7024.21</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>7024.06</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>7012.13</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>7010.5941164</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>6977.92</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>6985.03</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>7007.79</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>6962.92</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>6980.79</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>6988.67</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>7012.89</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>6985.24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-1787652128"/>
-        <c:axId val="-1787650352"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="-1787652128"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="yyyy/mm/dd\ hh:mm:ss" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1787650352"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-1787650352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1787652128"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3575,7 +549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3589,57 +563,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="str">
+      <c r="A1" s="15" t="str">
         <f>CONCATENATE("Bitcoin Performance over Time (", data!C2, ")")</f>
         <v>Bitcoin Performance over Time ($)</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="str">
+      <c r="A2" s="16" t="str">
         <f>CONCATENATE(TEXT(F4,"m/d/YYYY")," to ", TEXT(I4,"m/d/YYYY"))</f>
         <v>3/30/2018 to 4/2/2018</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <f>COUNT(data!B:B)</f>
         <v>365</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <f>MIN(data!A:A)</f>
         <v>43189.0056944444</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <f>MAX(data!A:A)</f>
         <v>43192.797488425902</v>
       </c>
@@ -3655,26 +629,26 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <f>AVERAGE(data!B:B)</f>
         <v>6928.2274538676766</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <f>MEDIAN(data!B:B)</f>
         <v>6948.94</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="10" t="str">
+      <c r="I6" s="8" t="str">
         <f>IF(1=1,"BUY","SELL")</f>
         <v>BUY</v>
       </c>
@@ -3690,26 +664,26 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <f>MIN(data!B:B)</f>
         <v>6493.16</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <f>MAX(data!B:B)</f>
         <v>7264.53</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="12" t="str">
+      <c r="I8" s="10" t="str">
         <f>IF(I6="BUY","HYPE","IT'S WORTH 0")</f>
         <v>HYPE</v>
       </c>
@@ -3722,12 +696,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E366"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>